<commit_message>
updared code for more improved code
</commit_message>
<xml_diff>
--- a/src/test/resources/IntelligentSearchQueries.xlsx
+++ b/src/test/resources/IntelligentSearchQueries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IntelligentSearchProject\search\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7531A7B8-A8A8-4B2C-9E6F-1E6F87D2E7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EE69E0-5B89-4A44-B714-D80B4A1D9438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{220C381F-5F09-4B15-A04E-C254D22CA39D}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Medtronics " sheetId="2" r:id="rId3"/>
     <sheet name="Terumo" sheetId="3" r:id="rId4"/>
     <sheet name="Crane1" sheetId="4" r:id="rId5"/>
+    <sheet name="Generic" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Number</t>
   </si>
@@ -104,6 +105,18 @@
   </si>
   <si>
     <t>401 optics initialization error</t>
+  </si>
+  <si>
+    <t>4012 optics initialization error .</t>
+  </si>
+  <si>
+    <t>device not starting</t>
+  </si>
+  <si>
+    <t>hardware failure</t>
+  </si>
+  <si>
+    <t>optics initialization error</t>
   </si>
 </sst>
 </file>
@@ -548,7 +561,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,7 +680,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,8 +738,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C1:U1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,4 +790,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101E0A02-5825-4F36-9557-51C8ECA9EC1E}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update new code for V1
</commit_message>
<xml_diff>
--- a/src/test/resources/IntelligentSearchQueries.xlsx
+++ b/src/test/resources/IntelligentSearchQueries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IntelligentSearchProject\search\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246CF6BC-E8B5-474C-A1EB-B7EF055DF094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108A8C80-1D6A-48F4-A144-A87DA1EA6C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{220C381F-5F09-4B15-A04E-C254D22CA39D}"/>
   </bookViews>
@@ -502,7 +502,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,7 +680,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,7 +797,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>